<commit_message>
renamed a couple of subNodes. Finished SignUp Page (hopefully)
</commit_message>
<xml_diff>
--- a/src/main/java/testData/Accounts.xlsx
+++ b/src/main/java/testData/Accounts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>QAZxsw123</t>
   </si>
@@ -42,13 +42,7 @@
     <t>Test</t>
   </si>
   <si>
-    <t>QAZxsw124</t>
-  </si>
-  <si>
-    <t>23xddsss</t>
-  </si>
-  <si>
-    <t>dsa3lx</t>
+    <t>23xddsss43</t>
   </si>
 </sst>
 </file>
@@ -366,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -396,7 +390,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -405,20 +399,6 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added the (automatic) Retry mechanism via the AnnotationTransformer.class
</commit_message>
<xml_diff>
--- a/src/main/java/testData/Accounts.xlsx
+++ b/src/main/java/testData/Accounts.xlsx
@@ -42,7 +42,7 @@
     <t>Test</t>
   </si>
   <si>
-    <t>23xddsss43</t>
+    <t>23xd43</t>
   </si>
 </sst>
 </file>
@@ -363,7 +363,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added more info in the report dashboard finished LoginPageTest
</commit_message>
<xml_diff>
--- a/src/main/java/testData/Accounts.xlsx
+++ b/src/main/java/testData/Accounts.xlsx
@@ -42,7 +42,7 @@
     <t>Test</t>
   </si>
   <si>
-    <t>23xd43</t>
+    <t>23xd43x</t>
   </si>
 </sst>
 </file>
@@ -363,7 +363,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Refactored registeredNewAccount from SignUpPageTest
</commit_message>
<xml_diff>
--- a/src/main/java/testData/Accounts.xlsx
+++ b/src/main/java/testData/Accounts.xlsx
@@ -42,7 +42,7 @@
     <t>Test</t>
   </si>
   <si>
-    <t>23xd43x</t>
+    <t>22dedas</t>
   </si>
 </sst>
 </file>
@@ -363,7 +363,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added more negative test to Create a new folder functionality in LibraryPage
</commit_message>
<xml_diff>
--- a/src/main/java/testData/Accounts.xlsx
+++ b/src/main/java/testData/Accounts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>email</t>
   </si>
@@ -36,7 +36,22 @@
     <t>Test</t>
   </si>
   <si>
-    <t>idj2jd92j</t>
+    <t>flirtest4</t>
+  </si>
+  <si>
+    <t>flirtest5</t>
+  </si>
+  <si>
+    <t>flirtest6</t>
+  </si>
+  <si>
+    <t>flirtest7</t>
+  </si>
+  <si>
+    <t>flirtest8</t>
+  </si>
+  <si>
+    <t>flirtest9</t>
   </si>
 </sst>
 </file>
@@ -354,20 +369,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -378,7 +393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -386,6 +401,61 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>